<commit_message>
generate charts from the results
</commit_message>
<xml_diff>
--- a/L1-Ergebnisse-Edge.xlsx
+++ b/L1-Ergebnisse-Edge.xlsx
@@ -8,13 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\IdeaProjects\F\Frezze_Tag_Problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D945A2-6FAC-458A-A5DF-F32F0BDBAAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3166D39C-185B-4A1E-9C09-5FCB54B730E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ergebnisse" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Ergebnisse!$I$2:$I$181</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Ergebnisse!$J$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Ergebnisse!$K$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Ergebnisse!$K$2:$K$181</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Ergebnisse!$L$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Ergebnisse!$L$2:$L$181</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Ergebnisse!$J$2:$J$181</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Ergebnisse!$K$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Ergebnisse!$K$2:$K$181</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Ergebnisse!$L$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Ergebnisse!$L$2:$L$181</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Ergebnisse!$I$2:$I$181</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Ergebnisse!$J$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Ergebnisse!$J$2:$J$181</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -106,6 +122,838 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.4</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.6</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Vergleich FTP-Algorithmen in L1 - Randdaten </cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1" compatLnSpc="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+            </a:rPr>
+            <a:t>Vergleich FTP-Algorithmen in L1 - Randdaten </a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{8F7002AE-F8F0-456A-AD13-007DC82D7055}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:v>best_next_aktive_robot</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{87AC5270-81BD-4B1A-BC54-C7F7D2B64A75}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:v>on_roboter_permutation</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{2AFE2329-D45D-46DA-83C3-A509A1CCACCD}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:v>greedy</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Anzahl Roboter</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+                </a:rPr>
+                <a:t>Anzahl Roboter</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:rich>
+              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Approximationsfaktor</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+                </a:endParaRPr>
+              </a:p>
+            </cx:rich>
+          </cx:tx>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>339725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Diagramm 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A6D38E3-79A2-0F87-9EA1-8378BA4E09D7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3082925" y="365125"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100"/>
+                <a:t>Dieses Diagramm ist in Ihrer Version von Excel nicht verfügbar.
+Wenn Sie diese Form bearbeiten oder diese Arbeitsmappe in einem anderen Dateiformat speichern, wird das Diagramm dauerhaft beschädigt.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,7 +1276,7 @@
   <dimension ref="A1:L181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7310,5 +8158,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>